<commit_message>
change to stancy succeeded gold0 100 cases auto antonym model
</commit_message>
<xml_diff>
--- a/Dataset/manul_opposite/stancy_100_gold0/stancy_succeeded_100_gold0.xlsx
+++ b/Dataset/manul_opposite/stancy_100_gold0/stancy_succeeded_100_gold0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Jupyter\stance_code\Dataset\manul_opposite\stancy_100_gold0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7570BE25-220D-4D5D-A321-4D6C1AFA9DA6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1A6EE56-7ABA-47A5-B369-D30B208B7A98}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25840" windowHeight="14027" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="226">
   <si>
     <t>Label</t>
   </si>
@@ -408,6 +408,394 @@
   </si>
   <si>
     <t>There are enough funding...</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>There are no cases where leaving school early is necessary</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Forced education achieves a lot</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>A lot is accomplished when education is forced.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Education that is forced does a lot.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>All skills are best learnt in a classroom environment.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Some skills are better learned inside the classroom.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>The classroom environment is ideal for all lessons.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Young people should not have the choice to decide for themselves</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Young people should not have the freedom to make their own choices.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Young people should not be able to think for themselves and make their own decisions.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Realistically cost</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Everyone is good at studying</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Most people are able to handle the rigor of university-level coursework.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>We should force people to study even if they aren't good at it and choose not to.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Everyone is good academically</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Most people are good at studying</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Compulsory studying would not be taking young people out of the workforce</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Making university education compulsory would not take young people out of the workforce.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>No young people would be taken out of workforce by compulsory studying</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>compulsory studying does not remove young people from the workforce</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Funding for museums is not wasteful</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>We should expect the state to fund museums</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>If state-funded, there is much incentive to increase numbers of visitors</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Opening up the Olympics for borderline sports is good in itself</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Chess has the necessary physical activity</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Chess can ensure fair play</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Federal States don't often have persistent losers.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Winners abound in federal states.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Positive discrimination towards women should be allowed</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>It is Women, Not Men, who are Disadvantaged in our Society</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Will not Cause Resentment Between Men and Women</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>It does address the underlying issues</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Positive discrimination for women is not discrimination</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>All-women shortlists or quotas have a constituent's freedom of choice</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Positive discrimination does not take away voters' freedom of choice by limiting their choices to women</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Some argue that a college education may be necessary even there are many people who have succeeded despite not having college degrees. </t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>The question of whether or not a college education is necessary for success is one that is not debated, even many successful people are not college educated.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Many people with college degrees find themselves working in positions in which their degrees are a requirement. </t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Colleges may be educating students instead of indoctrinating them.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Colleges may be helping them further their education rather than brainwashing their students.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Even too many students earning degrees has not diluted the value of a bachelor's degree.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>The value of a bachelor's degree has not lessened.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Few recent college graduates are un- or underemployed.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">In recent times, there aren't significant numbers of unemployed and underemployed college graduates. </t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>A college degree is guarantee of workplace benefits.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>There is guarantee there will be benefits.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Learning a trade profession is a worse option than college for many young adults.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>The total cost of going to college does not include the cost of missing opportunities to make money at a job.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>College stress can not lead to health problems and other negative consequences.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>College degrees do guarantee learning or job preparation.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Acquiring a degree does guarantee you a job.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Universities have unlimited places available</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Socialism has not changed historically to meet the challenges of the moment and is not addressing those of the 21st century in new ways</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Socialism can not be molded to fit the needs of the moment. </t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Socialism is not an ever changing set of principles that can be applied in new ways to meet the challenges of a changing world.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>socialism have not changed and adapted to meet the upcoming challenges of the 21st century</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Socialism is a less secure system than the free market in Capitalism</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Capitalism outranks Socialism in security.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>The proposed playoff system alternatives are actually more fair than the BCS system in place.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Historical evidence has shown that privatisation has been successful</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Full of trust</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>There is a lot of trust</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Agencies do not use surveillance to abuse their power.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gain of Privacy</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>People will not lose their privacy.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Privacy will not go away.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fighting bulls have a worse quality of life than meat-producing bulls</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>It would not create instability and logistical problems</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>The concept underestimates the role of the Prime Minister</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Puerto Rican statehood is economical for the US</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Puerto Rican statehood will benefit the US economically.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Making Puerto Rico a state is a good economic decision for the US. </t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Becoming a state would not hurt the other 50 states.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>God' is not a concept designed to promote a set of values</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>People think that a benevolent God can exist because bad things happen...</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>We should allow state sponsored revenge</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>There is not enough leeway in the law of self defence.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Animal researchers treat animals unhumanely, neither for the animals' sake nor to ensure reliable test results.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Animals are treated badly during animal testing. </t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Research animals are badly treated </t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Animals do have rights, therefore it is unacceptable to experiment on them.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Animals do have rights.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Testing is not needed for really new drugs</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">We do not need to be able to test drugs on animals.  </t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">We never use animal testing even when it is needed.  </t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Sometimes we have other choices for Animal research, so we don't need to do some animal testing. </t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Animal research does not ensure greater safety for humans</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Animal testing has not contributed to many life-saving cures and treatments.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Animal research has not played a vital role in a great many of the major medical advances of the last century</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Animals themselves do not benefit from the results of animal testing.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Most animals that are used in scientific testing have worse lives. </t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Religious traditions do not allow for human dominion over animals.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Animals are not the only choice for testing. </t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Animals are not appropriate research subjects even they are similar to human beings in many ways. </t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Many plays lend themselves to video review</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>video can catch all plays at a game</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Instant replay is deceptive and not inconclusive</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -479,7 +867,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -487,6 +875,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -791,11 +1180,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="E101" sqref="E101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.35" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="4" max="4" width="26.77734375" customWidth="1"/>
+    <col min="5" max="5" width="49.88671875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
@@ -875,7 +1268,7 @@
         <v>11</v>
       </c>
       <c r="E3" t="s">
-        <v>12</v>
+        <v>129</v>
       </c>
       <c r="F3" t="s">
         <v>12</v>
@@ -907,7 +1300,7 @@
         <v>11</v>
       </c>
       <c r="E4" t="s">
-        <v>13</v>
+        <v>130</v>
       </c>
       <c r="F4" t="s">
         <v>13</v>
@@ -939,7 +1332,7 @@
         <v>11</v>
       </c>
       <c r="E5" t="s">
-        <v>14</v>
+        <v>131</v>
       </c>
       <c r="F5" t="s">
         <v>14</v>
@@ -971,7 +1364,7 @@
         <v>11</v>
       </c>
       <c r="E6" t="s">
-        <v>15</v>
+        <v>132</v>
       </c>
       <c r="F6" t="s">
         <v>15</v>
@@ -1003,7 +1396,7 @@
         <v>11</v>
       </c>
       <c r="E7" t="s">
-        <v>16</v>
+        <v>130</v>
       </c>
       <c r="F7" t="s">
         <v>16</v>
@@ -1035,7 +1428,7 @@
         <v>11</v>
       </c>
       <c r="E8" t="s">
-        <v>17</v>
+        <v>133</v>
       </c>
       <c r="F8" t="s">
         <v>17</v>
@@ -1067,7 +1460,7 @@
         <v>11</v>
       </c>
       <c r="E9" t="s">
-        <v>18</v>
+        <v>134</v>
       </c>
       <c r="F9" t="s">
         <v>18</v>
@@ -1099,7 +1492,7 @@
         <v>11</v>
       </c>
       <c r="E10" t="s">
-        <v>19</v>
+        <v>135</v>
       </c>
       <c r="F10" t="s">
         <v>19</v>
@@ -1131,7 +1524,7 @@
         <v>11</v>
       </c>
       <c r="E11" t="s">
-        <v>20</v>
+        <v>136</v>
       </c>
       <c r="F11" t="s">
         <v>20</v>
@@ -1163,7 +1556,7 @@
         <v>11</v>
       </c>
       <c r="E12" t="s">
-        <v>21</v>
+        <v>137</v>
       </c>
       <c r="F12" t="s">
         <v>21</v>
@@ -1195,7 +1588,7 @@
         <v>11</v>
       </c>
       <c r="E13" t="s">
-        <v>22</v>
+        <v>138</v>
       </c>
       <c r="F13" t="s">
         <v>22</v>
@@ -1227,7 +1620,7 @@
         <v>11</v>
       </c>
       <c r="E14" t="s">
-        <v>23</v>
+        <v>139</v>
       </c>
       <c r="F14" t="s">
         <v>23</v>
@@ -1259,7 +1652,7 @@
         <v>11</v>
       </c>
       <c r="E15" t="s">
-        <v>24</v>
+        <v>140</v>
       </c>
       <c r="F15" t="s">
         <v>24</v>
@@ -1291,7 +1684,7 @@
         <v>11</v>
       </c>
       <c r="E16" t="s">
-        <v>25</v>
+        <v>141</v>
       </c>
       <c r="F16" t="s">
         <v>25</v>
@@ -1323,7 +1716,7 @@
         <v>11</v>
       </c>
       <c r="E17" t="s">
-        <v>26</v>
+        <v>142</v>
       </c>
       <c r="F17" t="s">
         <v>26</v>
@@ -1355,7 +1748,7 @@
         <v>11</v>
       </c>
       <c r="E18" t="s">
-        <v>27</v>
+        <v>143</v>
       </c>
       <c r="F18" t="s">
         <v>27</v>
@@ -1387,7 +1780,7 @@
         <v>11</v>
       </c>
       <c r="E19" t="s">
-        <v>28</v>
+        <v>144</v>
       </c>
       <c r="F19" t="s">
         <v>28</v>
@@ -1419,7 +1812,7 @@
         <v>11</v>
       </c>
       <c r="E20" t="s">
-        <v>29</v>
+        <v>145</v>
       </c>
       <c r="F20" t="s">
         <v>29</v>
@@ -1451,7 +1844,7 @@
         <v>11</v>
       </c>
       <c r="E21" t="s">
-        <v>30</v>
+        <v>146</v>
       </c>
       <c r="F21" t="s">
         <v>30</v>
@@ -1483,7 +1876,7 @@
         <v>11</v>
       </c>
       <c r="E22" t="s">
-        <v>31</v>
+        <v>147</v>
       </c>
       <c r="F22" t="s">
         <v>31</v>
@@ -1515,7 +1908,7 @@
         <v>11</v>
       </c>
       <c r="E23" t="s">
-        <v>32</v>
+        <v>148</v>
       </c>
       <c r="F23" t="s">
         <v>32</v>
@@ -1547,7 +1940,7 @@
         <v>33</v>
       </c>
       <c r="E24" t="s">
-        <v>34</v>
+        <v>149</v>
       </c>
       <c r="F24" t="s">
         <v>34</v>
@@ -1579,7 +1972,7 @@
         <v>33</v>
       </c>
       <c r="E25" t="s">
-        <v>35</v>
+        <v>150</v>
       </c>
       <c r="F25" t="s">
         <v>35</v>
@@ -1611,7 +2004,7 @@
         <v>33</v>
       </c>
       <c r="E26" t="s">
-        <v>36</v>
+        <v>151</v>
       </c>
       <c r="F26" t="s">
         <v>36</v>
@@ -1643,7 +2036,7 @@
         <v>37</v>
       </c>
       <c r="E27" t="s">
-        <v>38</v>
+        <v>152</v>
       </c>
       <c r="F27" t="s">
         <v>38</v>
@@ -1675,7 +2068,7 @@
         <v>37</v>
       </c>
       <c r="E28" t="s">
-        <v>39</v>
+        <v>153</v>
       </c>
       <c r="F28" t="s">
         <v>39</v>
@@ -1707,7 +2100,7 @@
         <v>37</v>
       </c>
       <c r="E29" t="s">
-        <v>40</v>
+        <v>154</v>
       </c>
       <c r="F29" t="s">
         <v>40</v>
@@ -1739,7 +2132,7 @@
         <v>41</v>
       </c>
       <c r="E30" t="s">
-        <v>42</v>
+        <v>155</v>
       </c>
       <c r="F30" t="s">
         <v>42</v>
@@ -1771,7 +2164,7 @@
         <v>41</v>
       </c>
       <c r="E31" t="s">
-        <v>43</v>
+        <v>156</v>
       </c>
       <c r="F31" t="s">
         <v>43</v>
@@ -1803,7 +2196,7 @@
         <v>44</v>
       </c>
       <c r="E32" t="s">
-        <v>45</v>
+        <v>157</v>
       </c>
       <c r="F32" t="s">
         <v>45</v>
@@ -1835,7 +2228,7 @@
         <v>44</v>
       </c>
       <c r="E33" t="s">
-        <v>46</v>
+        <v>158</v>
       </c>
       <c r="F33" t="s">
         <v>46</v>
@@ -1867,7 +2260,7 @@
         <v>44</v>
       </c>
       <c r="E34" t="s">
-        <v>47</v>
+        <v>159</v>
       </c>
       <c r="F34" t="s">
         <v>47</v>
@@ -1899,7 +2292,7 @@
         <v>44</v>
       </c>
       <c r="E35" t="s">
-        <v>48</v>
+        <v>160</v>
       </c>
       <c r="F35" t="s">
         <v>48</v>
@@ -1931,7 +2324,7 @@
         <v>44</v>
       </c>
       <c r="E36" t="s">
-        <v>49</v>
+        <v>161</v>
       </c>
       <c r="F36" t="s">
         <v>49</v>
@@ -1963,7 +2356,7 @@
         <v>44</v>
       </c>
       <c r="E37" t="s">
-        <v>50</v>
+        <v>162</v>
       </c>
       <c r="F37" t="s">
         <v>50</v>
@@ -1995,7 +2388,7 @@
         <v>44</v>
       </c>
       <c r="E38" t="s">
-        <v>51</v>
+        <v>163</v>
       </c>
       <c r="F38" t="s">
         <v>51</v>
@@ -2027,7 +2420,7 @@
         <v>52</v>
       </c>
       <c r="E39" t="s">
-        <v>53</v>
+        <v>164</v>
       </c>
       <c r="F39" t="s">
         <v>53</v>
@@ -2059,7 +2452,7 @@
         <v>52</v>
       </c>
       <c r="E40" t="s">
-        <v>54</v>
+        <v>165</v>
       </c>
       <c r="F40" t="s">
         <v>54</v>
@@ -2091,7 +2484,7 @@
         <v>52</v>
       </c>
       <c r="E41" t="s">
-        <v>55</v>
+        <v>166</v>
       </c>
       <c r="F41" t="s">
         <v>55</v>
@@ -2123,7 +2516,7 @@
         <v>52</v>
       </c>
       <c r="E42" t="s">
-        <v>56</v>
+        <v>167</v>
       </c>
       <c r="F42" t="s">
         <v>56</v>
@@ -2155,7 +2548,7 @@
         <v>52</v>
       </c>
       <c r="E43" t="s">
-        <v>57</v>
+        <v>168</v>
       </c>
       <c r="F43" t="s">
         <v>57</v>
@@ -2187,7 +2580,7 @@
         <v>52</v>
       </c>
       <c r="E44" t="s">
-        <v>58</v>
+        <v>169</v>
       </c>
       <c r="F44" t="s">
         <v>58</v>
@@ -2219,7 +2612,7 @@
         <v>52</v>
       </c>
       <c r="E45" t="s">
-        <v>59</v>
+        <v>170</v>
       </c>
       <c r="F45" t="s">
         <v>59</v>
@@ -2251,7 +2644,7 @@
         <v>52</v>
       </c>
       <c r="E46" t="s">
-        <v>60</v>
+        <v>171</v>
       </c>
       <c r="F46" t="s">
         <v>60</v>
@@ -2283,7 +2676,7 @@
         <v>52</v>
       </c>
       <c r="E47" t="s">
-        <v>61</v>
+        <v>172</v>
       </c>
       <c r="F47" t="s">
         <v>61</v>
@@ -2315,7 +2708,7 @@
         <v>52</v>
       </c>
       <c r="E48" t="s">
-        <v>62</v>
+        <v>173</v>
       </c>
       <c r="F48" t="s">
         <v>62</v>
@@ -2347,7 +2740,7 @@
         <v>52</v>
       </c>
       <c r="E49" t="s">
-        <v>63</v>
+        <v>174</v>
       </c>
       <c r="F49" t="s">
         <v>63</v>
@@ -2379,7 +2772,7 @@
         <v>52</v>
       </c>
       <c r="E50" t="s">
-        <v>64</v>
+        <v>175</v>
       </c>
       <c r="F50" t="s">
         <v>64</v>
@@ -2411,7 +2804,7 @@
         <v>52</v>
       </c>
       <c r="E51" t="s">
-        <v>65</v>
+        <v>176</v>
       </c>
       <c r="F51" t="s">
         <v>65</v>
@@ -2443,7 +2836,7 @@
         <v>52</v>
       </c>
       <c r="E52" t="s">
-        <v>66</v>
+        <v>177</v>
       </c>
       <c r="F52" t="s">
         <v>66</v>
@@ -2475,7 +2868,7 @@
         <v>52</v>
       </c>
       <c r="E53" t="s">
-        <v>67</v>
+        <v>178</v>
       </c>
       <c r="F53" t="s">
         <v>67</v>
@@ -2507,7 +2900,7 @@
         <v>52</v>
       </c>
       <c r="E54" t="s">
-        <v>68</v>
+        <v>179</v>
       </c>
       <c r="F54" t="s">
         <v>68</v>
@@ -2539,7 +2932,7 @@
         <v>52</v>
       </c>
       <c r="E55" t="s">
-        <v>69</v>
+        <v>180</v>
       </c>
       <c r="F55" t="s">
         <v>69</v>
@@ -2571,7 +2964,7 @@
         <v>70</v>
       </c>
       <c r="E56" t="s">
-        <v>71</v>
+        <v>181</v>
       </c>
       <c r="F56" t="s">
         <v>71</v>
@@ -2603,7 +2996,7 @@
         <v>70</v>
       </c>
       <c r="E57" t="s">
-        <v>72</v>
+        <v>182</v>
       </c>
       <c r="F57" t="s">
         <v>72</v>
@@ -2635,7 +3028,7 @@
         <v>70</v>
       </c>
       <c r="E58" t="s">
-        <v>73</v>
+        <v>183</v>
       </c>
       <c r="F58" t="s">
         <v>73</v>
@@ -2667,7 +3060,7 @@
         <v>70</v>
       </c>
       <c r="E59" t="s">
-        <v>74</v>
+        <v>184</v>
       </c>
       <c r="F59" t="s">
         <v>74</v>
@@ -2699,7 +3092,7 @@
         <v>70</v>
       </c>
       <c r="E60" t="s">
-        <v>75</v>
+        <v>185</v>
       </c>
       <c r="F60" t="s">
         <v>75</v>
@@ -2731,7 +3124,7 @@
         <v>70</v>
       </c>
       <c r="E61" t="s">
-        <v>76</v>
+        <v>186</v>
       </c>
       <c r="F61" t="s">
         <v>76</v>
@@ -2763,7 +3156,7 @@
         <v>77</v>
       </c>
       <c r="E62" t="s">
-        <v>78</v>
+        <v>187</v>
       </c>
       <c r="F62" t="s">
         <v>78</v>
@@ -2795,7 +3188,7 @@
         <v>79</v>
       </c>
       <c r="E63" t="s">
-        <v>80</v>
+        <v>188</v>
       </c>
       <c r="F63" t="s">
         <v>80</v>
@@ -2827,7 +3220,7 @@
         <v>81</v>
       </c>
       <c r="E64" t="s">
-        <v>82</v>
+        <v>189</v>
       </c>
       <c r="F64" t="s">
         <v>82</v>
@@ -2859,7 +3252,7 @@
         <v>81</v>
       </c>
       <c r="E65" t="s">
-        <v>83</v>
+        <v>190</v>
       </c>
       <c r="F65" t="s">
         <v>83</v>
@@ -2891,7 +3284,7 @@
         <v>81</v>
       </c>
       <c r="E66" t="s">
-        <v>84</v>
+        <v>191</v>
       </c>
       <c r="F66" t="s">
         <v>84</v>
@@ -2923,7 +3316,7 @@
         <v>81</v>
       </c>
       <c r="E67" t="s">
-        <v>85</v>
+        <v>192</v>
       </c>
       <c r="F67" t="s">
         <v>85</v>
@@ -2955,7 +3348,7 @@
         <v>81</v>
       </c>
       <c r="E68" t="s">
-        <v>86</v>
+        <v>193</v>
       </c>
       <c r="F68" t="s">
         <v>86</v>
@@ -2987,7 +3380,7 @@
         <v>81</v>
       </c>
       <c r="E69" t="s">
-        <v>87</v>
+        <v>194</v>
       </c>
       <c r="F69" t="s">
         <v>87</v>
@@ -3019,7 +3412,7 @@
         <v>88</v>
       </c>
       <c r="E70" t="s">
-        <v>89</v>
+        <v>195</v>
       </c>
       <c r="F70" t="s">
         <v>89</v>
@@ -3051,7 +3444,7 @@
         <v>90</v>
       </c>
       <c r="E71" t="s">
-        <v>91</v>
+        <v>196</v>
       </c>
       <c r="F71" t="s">
         <v>91</v>
@@ -3083,7 +3476,7 @@
         <v>90</v>
       </c>
       <c r="E72" t="s">
-        <v>92</v>
+        <v>197</v>
       </c>
       <c r="F72" t="s">
         <v>92</v>
@@ -3115,7 +3508,7 @@
         <v>93</v>
       </c>
       <c r="E73" t="s">
-        <v>94</v>
+        <v>198</v>
       </c>
       <c r="F73" t="s">
         <v>94</v>
@@ -3147,7 +3540,7 @@
         <v>93</v>
       </c>
       <c r="E74" t="s">
-        <v>95</v>
+        <v>199</v>
       </c>
       <c r="F74" t="s">
         <v>95</v>
@@ -3179,7 +3572,7 @@
         <v>93</v>
       </c>
       <c r="E75" t="s">
-        <v>96</v>
+        <v>200</v>
       </c>
       <c r="F75" t="s">
         <v>96</v>
@@ -3211,7 +3604,7 @@
         <v>93</v>
       </c>
       <c r="E76" t="s">
-        <v>97</v>
+        <v>201</v>
       </c>
       <c r="F76" t="s">
         <v>97</v>
@@ -3242,8 +3635,8 @@
       <c r="D77" t="s">
         <v>98</v>
       </c>
-      <c r="E77" t="s">
-        <v>99</v>
+      <c r="E77" s="3" t="s">
+        <v>202</v>
       </c>
       <c r="F77" t="s">
         <v>99</v>
@@ -3275,7 +3668,7 @@
         <v>98</v>
       </c>
       <c r="E78" t="s">
-        <v>100</v>
+        <v>203</v>
       </c>
       <c r="F78" t="s">
         <v>100</v>
@@ -3307,7 +3700,7 @@
         <v>101</v>
       </c>
       <c r="E79" t="s">
-        <v>102</v>
+        <v>204</v>
       </c>
       <c r="F79" t="s">
         <v>102</v>
@@ -3339,7 +3732,7 @@
         <v>101</v>
       </c>
       <c r="E80" t="s">
-        <v>103</v>
+        <v>205</v>
       </c>
       <c r="F80" t="s">
         <v>103</v>
@@ -3371,7 +3764,7 @@
         <v>104</v>
       </c>
       <c r="E81" t="s">
-        <v>105</v>
+        <v>206</v>
       </c>
       <c r="F81" t="s">
         <v>105</v>
@@ -3403,7 +3796,7 @@
         <v>104</v>
       </c>
       <c r="E82" t="s">
-        <v>106</v>
+        <v>207</v>
       </c>
       <c r="F82" t="s">
         <v>106</v>
@@ -3435,7 +3828,7 @@
         <v>104</v>
       </c>
       <c r="E83" t="s">
-        <v>107</v>
+        <v>208</v>
       </c>
       <c r="F83" t="s">
         <v>107</v>
@@ -3467,7 +3860,7 @@
         <v>104</v>
       </c>
       <c r="E84" t="s">
-        <v>108</v>
+        <v>209</v>
       </c>
       <c r="F84" t="s">
         <v>108</v>
@@ -3499,7 +3892,7 @@
         <v>104</v>
       </c>
       <c r="E85" t="s">
-        <v>109</v>
+        <v>210</v>
       </c>
       <c r="F85" t="s">
         <v>109</v>
@@ -3531,7 +3924,7 @@
         <v>104</v>
       </c>
       <c r="E86" t="s">
-        <v>110</v>
+        <v>211</v>
       </c>
       <c r="F86" t="s">
         <v>110</v>
@@ -3563,7 +3956,7 @@
         <v>104</v>
       </c>
       <c r="E87" t="s">
-        <v>111</v>
+        <v>212</v>
       </c>
       <c r="F87" t="s">
         <v>111</v>
@@ -3595,7 +3988,7 @@
         <v>104</v>
       </c>
       <c r="E88" t="s">
-        <v>112</v>
+        <v>213</v>
       </c>
       <c r="F88" t="s">
         <v>112</v>
@@ -3627,7 +4020,7 @@
         <v>104</v>
       </c>
       <c r="E89" t="s">
-        <v>113</v>
+        <v>214</v>
       </c>
       <c r="F89" t="s">
         <v>113</v>
@@ -3659,7 +4052,7 @@
         <v>104</v>
       </c>
       <c r="E90" t="s">
-        <v>114</v>
+        <v>215</v>
       </c>
       <c r="F90" t="s">
         <v>114</v>
@@ -3691,7 +4084,7 @@
         <v>104</v>
       </c>
       <c r="E91" t="s">
-        <v>115</v>
+        <v>216</v>
       </c>
       <c r="F91" t="s">
         <v>115</v>
@@ -3723,7 +4116,7 @@
         <v>104</v>
       </c>
       <c r="E92" t="s">
-        <v>116</v>
+        <v>217</v>
       </c>
       <c r="F92" t="s">
         <v>116</v>
@@ -3787,7 +4180,7 @@
         <v>104</v>
       </c>
       <c r="E94" t="s">
-        <v>118</v>
+        <v>218</v>
       </c>
       <c r="F94" t="s">
         <v>118</v>
@@ -3819,7 +4212,7 @@
         <v>104</v>
       </c>
       <c r="E95" t="s">
-        <v>119</v>
+        <v>219</v>
       </c>
       <c r="F95" t="s">
         <v>119</v>
@@ -3851,7 +4244,7 @@
         <v>104</v>
       </c>
       <c r="E96" t="s">
-        <v>120</v>
+        <v>220</v>
       </c>
       <c r="F96" t="s">
         <v>120</v>
@@ -3883,7 +4276,7 @@
         <v>104</v>
       </c>
       <c r="E97" t="s">
-        <v>121</v>
+        <v>221</v>
       </c>
       <c r="F97" t="s">
         <v>121</v>
@@ -3915,7 +4308,7 @@
         <v>104</v>
       </c>
       <c r="E98" t="s">
-        <v>122</v>
+        <v>222</v>
       </c>
       <c r="F98" t="s">
         <v>122</v>
@@ -3947,7 +4340,7 @@
         <v>123</v>
       </c>
       <c r="E99" t="s">
-        <v>124</v>
+        <v>223</v>
       </c>
       <c r="F99" t="s">
         <v>124</v>
@@ -3979,7 +4372,7 @@
         <v>123</v>
       </c>
       <c r="E100" t="s">
-        <v>125</v>
+        <v>224</v>
       </c>
       <c r="F100" t="s">
         <v>125</v>
@@ -4011,7 +4404,7 @@
         <v>123</v>
       </c>
       <c r="E101" t="s">
-        <v>126</v>
+        <v>225</v>
       </c>
       <c r="F101" t="s">
         <v>126</v>

</xml_diff>